<commit_message>
fix(precios): fixed precios and product images
</commit_message>
<xml_diff>
--- a/descargas/precios_medios_2025.xlsx
+++ b/descargas/precios_medios_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\10 Precios coyunturales\3 Informes y Resultados\ISC\Semana 2512\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\10 Precios coyunturales\3 Informes y Resultados\ISC\Semana 2519\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458E53D4-540B-4EA9-9575-09529AB62F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27850D50-D232-47D8-A96A-1C2573BF0C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B7F45DA3-520B-4C64-92AB-DC7769421BDC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7F45DA3-520B-4C64-92AB-DC7769421BDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Precios semanales " sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="226">
   <si>
     <t>PRECIOS MEDIOS NACIONALES</t>
   </si>
@@ -675,6 +675,48 @@
   </si>
   <si>
     <t>17/03 - 23/03</t>
+  </si>
+  <si>
+    <t>Semana 13</t>
+  </si>
+  <si>
+    <t>24/03 - 30/03</t>
+  </si>
+  <si>
+    <t>Semana 14</t>
+  </si>
+  <si>
+    <t>31/03 - 06/04</t>
+  </si>
+  <si>
+    <t>07/04 - 13/04</t>
+  </si>
+  <si>
+    <t>Semana 15</t>
+  </si>
+  <si>
+    <t>Semana 16</t>
+  </si>
+  <si>
+    <t>14/04 - 20/04</t>
+  </si>
+  <si>
+    <t>Semana 17</t>
+  </si>
+  <si>
+    <t>21/04 - 27/04</t>
+  </si>
+  <si>
+    <t>Semana 18</t>
+  </si>
+  <si>
+    <t>28/04 - 04/05</t>
+  </si>
+  <si>
+    <t>Semana 19</t>
+  </si>
+  <si>
+    <t>05/05 - 11/05</t>
   </si>
 </sst>
 </file>
@@ -1606,43 +1648,43 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O170"/>
+  <dimension ref="A1:V170"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <pane xSplit="3" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="20.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="56.77734375" style="45" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="69.6640625" style="2" customWidth="1"/>
-    <col min="4" max="15" width="17.21875" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="11.5546875" style="2"/>
+    <col min="1" max="1" width="56.7265625" style="45" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="69.7265625" style="2" customWidth="1"/>
+    <col min="4" max="22" width="17.26953125" style="2" customWidth="1"/>
+    <col min="23" max="16384" width="11.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="31.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:22" ht="32.5" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:22" ht="34.5" x14ac:dyDescent="0.65">
       <c r="A2" s="3">
         <v>2025</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A3" s="3"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:22" ht="22.5" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:15" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:22" ht="34.5" x14ac:dyDescent="0.65">
       <c r="A5" s="3"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -1656,8 +1698,15 @@
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
-    </row>
-    <row r="6" spans="1:15" s="8" customFormat="1" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+    </row>
+    <row r="6" spans="1:22" s="8" customFormat="1" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="7"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -1671,8 +1720,15 @@
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
-    </row>
-    <row r="7" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+    </row>
+    <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
@@ -1716,8 +1772,29 @@
       <c r="O7" s="11" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="P7" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="U7" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="V7" s="11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="12"/>
       <c r="B8" s="61" t="s">
         <v>5</v>
@@ -1759,8 +1836,29 @@
       <c r="O8" s="13" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P8" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="R8" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="S8" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="T8" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="U8" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="V8" s="13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="63" t="s">
         <v>6</v>
       </c>
@@ -1806,8 +1904,29 @@
       <c r="O9" s="16">
         <v>230.73</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P9" s="16">
+        <v>228.87</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>227.02</v>
+      </c>
+      <c r="R9" s="16">
+        <v>224.77</v>
+      </c>
+      <c r="S9" s="16">
+        <v>224.38</v>
+      </c>
+      <c r="T9" s="16">
+        <v>221.63</v>
+      </c>
+      <c r="U9" s="16">
+        <v>218.87</v>
+      </c>
+      <c r="V9" s="16">
+        <v>215.49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="64"/>
       <c r="B10" s="18" t="s">
         <v>7</v>
@@ -1851,8 +1970,29 @@
       <c r="O10" s="20">
         <v>286.76</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P10" s="20">
+        <v>286.76</v>
+      </c>
+      <c r="Q10" s="20">
+        <v>286.76</v>
+      </c>
+      <c r="R10" s="20">
+        <v>288.38</v>
+      </c>
+      <c r="S10" s="20">
+        <v>288.38</v>
+      </c>
+      <c r="T10" s="20">
+        <v>289.49</v>
+      </c>
+      <c r="U10" s="20">
+        <v>288.45999999999998</v>
+      </c>
+      <c r="V10" s="20">
+        <v>286.73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="64"/>
       <c r="B11" s="18" t="s">
         <v>7</v>
@@ -1896,8 +2036,29 @@
       <c r="O11" s="20">
         <v>212.64</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="20">
+        <v>211.35</v>
+      </c>
+      <c r="Q11" s="20">
+        <v>209.58</v>
+      </c>
+      <c r="R11" s="20">
+        <v>205.36</v>
+      </c>
+      <c r="S11" s="20">
+        <v>205.28</v>
+      </c>
+      <c r="T11" s="20">
+        <v>201.8</v>
+      </c>
+      <c r="U11" s="20">
+        <v>199.72</v>
+      </c>
+      <c r="V11" s="20">
+        <v>196.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="64"/>
       <c r="B12" s="18" t="s">
         <v>7</v>
@@ -1941,8 +2102,29 @@
       <c r="O12" s="20">
         <v>234.47</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P12" s="20">
+        <v>230.7</v>
+      </c>
+      <c r="Q12" s="20">
+        <v>229.02</v>
+      </c>
+      <c r="R12" s="20">
+        <v>226.44</v>
+      </c>
+      <c r="S12" s="20">
+        <v>226.44</v>
+      </c>
+      <c r="T12" s="20">
+        <v>224.39</v>
+      </c>
+      <c r="U12" s="20">
+        <v>222.39</v>
+      </c>
+      <c r="V12" s="20">
+        <v>220.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="64"/>
       <c r="B13" s="22" t="s">
         <v>7</v>
@@ -1986,8 +2168,29 @@
       <c r="O13" s="24">
         <v>239.46</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="24">
+        <v>236.53</v>
+      </c>
+      <c r="Q13" s="24">
+        <v>235.27</v>
+      </c>
+      <c r="R13" s="24">
+        <v>234.47</v>
+      </c>
+      <c r="S13" s="24">
+        <v>234.47</v>
+      </c>
+      <c r="T13" s="24">
+        <v>232.73</v>
+      </c>
+      <c r="U13" s="24">
+        <v>232.02</v>
+      </c>
+      <c r="V13" s="24">
+        <v>229.44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="63" t="s">
         <v>13</v>
       </c>
@@ -2033,8 +2236,29 @@
       <c r="O14" s="20">
         <v>528.9</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P14" s="20">
+        <v>528.9</v>
+      </c>
+      <c r="Q14" s="20">
+        <v>532.23</v>
+      </c>
+      <c r="R14" s="20">
+        <v>532.23</v>
+      </c>
+      <c r="S14" s="20">
+        <v>532.23</v>
+      </c>
+      <c r="T14" s="20">
+        <v>532.23</v>
+      </c>
+      <c r="U14" s="20">
+        <v>532.23</v>
+      </c>
+      <c r="V14" s="20">
+        <v>532.23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="64"/>
       <c r="B15" s="18" t="s">
         <v>14</v>
@@ -2078,8 +2302,29 @@
       <c r="O15" s="20">
         <v>462.68</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P15" s="20">
+        <v>462.68</v>
+      </c>
+      <c r="Q15" s="20">
+        <v>460.49</v>
+      </c>
+      <c r="R15" s="20">
+        <v>460.49</v>
+      </c>
+      <c r="S15" s="20">
+        <v>460.49</v>
+      </c>
+      <c r="T15" s="20">
+        <v>460.49</v>
+      </c>
+      <c r="U15" s="20">
+        <v>460.49</v>
+      </c>
+      <c r="V15" s="20">
+        <v>460.49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="64"/>
       <c r="B16" s="18" t="s">
         <v>17</v>
@@ -2123,8 +2368,29 @@
       <c r="O16" s="20">
         <v>1170.1199999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P16" s="20">
+        <v>1170.1199999999999</v>
+      </c>
+      <c r="Q16" s="20">
+        <v>1129.0899999999999</v>
+      </c>
+      <c r="R16" s="20">
+        <v>1129.0899999999999</v>
+      </c>
+      <c r="S16" s="20">
+        <v>1129.0899999999999</v>
+      </c>
+      <c r="T16" s="20">
+        <v>1129.0899999999999</v>
+      </c>
+      <c r="U16" s="20">
+        <v>1129.0899999999999</v>
+      </c>
+      <c r="V16" s="20">
+        <v>1129.0899999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="64"/>
       <c r="B17" s="18" t="s">
         <v>17</v>
@@ -2168,8 +2434,29 @@
       <c r="O17" s="20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P17" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q17" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="R17" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="S17" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="T17" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="U17" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="V17" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="64"/>
       <c r="B18" s="18" t="s">
         <v>17</v>
@@ -2213,8 +2500,29 @@
       <c r="O18" s="20">
         <v>498.81</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P18" s="20">
+        <v>498.81</v>
+      </c>
+      <c r="Q18" s="20">
+        <v>472.29</v>
+      </c>
+      <c r="R18" s="20">
+        <v>472.29</v>
+      </c>
+      <c r="S18" s="20">
+        <v>472.29</v>
+      </c>
+      <c r="T18" s="20">
+        <v>472.29</v>
+      </c>
+      <c r="U18" s="20">
+        <v>472.29</v>
+      </c>
+      <c r="V18" s="20">
+        <v>472.29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="65"/>
       <c r="B19" s="22" t="s">
         <v>17</v>
@@ -2258,8 +2566,29 @@
       <c r="O19" s="20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P19" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q19" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="R19" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="S19" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="T19" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="U19" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="V19" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="66" t="s">
         <v>22</v>
       </c>
@@ -2305,8 +2634,29 @@
       <c r="O20" s="17">
         <v>392.25</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P20" s="17">
+        <v>391.29</v>
+      </c>
+      <c r="Q20" s="17">
+        <v>390.45</v>
+      </c>
+      <c r="R20" s="17">
+        <v>391.24</v>
+      </c>
+      <c r="S20" s="17">
+        <v>396.43</v>
+      </c>
+      <c r="T20" s="17">
+        <v>390.28</v>
+      </c>
+      <c r="U20" s="17">
+        <v>377.07</v>
+      </c>
+      <c r="V20" s="17">
+        <v>370.52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="67"/>
       <c r="B21" s="28" t="s">
         <v>23</v>
@@ -2350,8 +2700,29 @@
       <c r="O21" s="21">
         <v>333.63</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P21" s="21">
+        <v>333.05</v>
+      </c>
+      <c r="Q21" s="21">
+        <v>331.96</v>
+      </c>
+      <c r="R21" s="21">
+        <v>333.48</v>
+      </c>
+      <c r="S21" s="21">
+        <v>335.98</v>
+      </c>
+      <c r="T21" s="21">
+        <v>330.27</v>
+      </c>
+      <c r="U21" s="21">
+        <v>330.27</v>
+      </c>
+      <c r="V21" s="21">
+        <v>312.52999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="67"/>
       <c r="B22" s="28" t="s">
         <v>23</v>
@@ -2395,8 +2766,29 @@
       <c r="O22" s="21">
         <v>303.91000000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P22" s="21">
+        <v>301.66000000000003</v>
+      </c>
+      <c r="Q22" s="21">
+        <v>297.93</v>
+      </c>
+      <c r="R22" s="21">
+        <v>298.08999999999997</v>
+      </c>
+      <c r="S22" s="21">
+        <v>300.61</v>
+      </c>
+      <c r="T22" s="21">
+        <v>295.87</v>
+      </c>
+      <c r="U22" s="21">
+        <v>295.24</v>
+      </c>
+      <c r="V22" s="21">
+        <v>270.27999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="67"/>
       <c r="B23" s="28" t="s">
         <v>27</v>
@@ -2440,8 +2832,29 @@
       <c r="O23" s="21">
         <v>336.44</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P23" s="21">
+        <v>337.4</v>
+      </c>
+      <c r="Q23" s="21">
+        <v>334.88</v>
+      </c>
+      <c r="R23" s="21">
+        <v>327.17</v>
+      </c>
+      <c r="S23" s="21">
+        <v>327.82</v>
+      </c>
+      <c r="T23" s="21">
+        <v>327.08</v>
+      </c>
+      <c r="U23" s="21">
+        <v>319.82</v>
+      </c>
+      <c r="V23" s="21">
+        <v>319.82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="67"/>
       <c r="B24" s="28" t="s">
         <v>29</v>
@@ -2485,8 +2898,29 @@
       <c r="O24" s="21">
         <v>136.03</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P24" s="21">
+        <v>132.12</v>
+      </c>
+      <c r="Q24" s="21">
+        <v>130.33000000000001</v>
+      </c>
+      <c r="R24" s="21">
+        <v>129.72999999999999</v>
+      </c>
+      <c r="S24" s="21">
+        <v>128.59</v>
+      </c>
+      <c r="T24" s="21">
+        <v>126.35</v>
+      </c>
+      <c r="U24" s="21">
+        <v>124.73</v>
+      </c>
+      <c r="V24" s="21">
+        <v>124.98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="67"/>
       <c r="B25" s="28" t="s">
         <v>27</v>
@@ -2530,8 +2964,29 @@
       <c r="O25" s="21">
         <v>239</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P25" s="21">
+        <v>238.83</v>
+      </c>
+      <c r="Q25" s="21">
+        <v>235.34</v>
+      </c>
+      <c r="R25" s="21">
+        <v>234.47</v>
+      </c>
+      <c r="S25" s="21">
+        <v>231.08</v>
+      </c>
+      <c r="T25" s="21">
+        <v>229.58</v>
+      </c>
+      <c r="U25" s="21">
+        <v>224.67</v>
+      </c>
+      <c r="V25" s="21">
+        <v>224.59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="67"/>
       <c r="B26" s="28" t="s">
         <v>27</v>
@@ -2575,8 +3030,29 @@
       <c r="O26" s="21">
         <v>129.68</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P26" s="21">
+        <v>129.66</v>
+      </c>
+      <c r="Q26" s="21">
+        <v>129.63999999999999</v>
+      </c>
+      <c r="R26" s="21">
+        <v>128.41999999999999</v>
+      </c>
+      <c r="S26" s="21">
+        <v>128.22999999999999</v>
+      </c>
+      <c r="T26" s="21">
+        <v>127.58</v>
+      </c>
+      <c r="U26" s="21">
+        <v>126.52</v>
+      </c>
+      <c r="V26" s="21">
+        <v>127.16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="67"/>
       <c r="B27" s="28" t="s">
         <v>27</v>
@@ -2620,8 +3096,29 @@
       <c r="O27" s="21">
         <v>166.61</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P27" s="21">
+        <v>166.77</v>
+      </c>
+      <c r="Q27" s="21">
+        <v>168.78</v>
+      </c>
+      <c r="R27" s="21">
+        <v>167.23</v>
+      </c>
+      <c r="S27" s="21">
+        <v>165.98</v>
+      </c>
+      <c r="T27" s="21">
+        <v>163.78</v>
+      </c>
+      <c r="U27" s="21">
+        <v>163.68</v>
+      </c>
+      <c r="V27" s="21">
+        <v>162.72999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="67"/>
       <c r="B28" s="28" t="s">
         <v>27</v>
@@ -2665,8 +3162,29 @@
       <c r="O28" s="21">
         <v>125.29549999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P28" s="21">
+        <v>125.96099999999998</v>
+      </c>
+      <c r="Q28" s="21">
+        <v>132.19819999999999</v>
+      </c>
+      <c r="R28" s="21">
+        <v>126.67229999999999</v>
+      </c>
+      <c r="S28" s="21">
+        <v>125.7286</v>
+      </c>
+      <c r="T28" s="21">
+        <v>122.85799999999999</v>
+      </c>
+      <c r="U28" s="21">
+        <v>127.52000000000001</v>
+      </c>
+      <c r="V28" s="21">
+        <v>124.7474</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="67"/>
       <c r="B29" s="28" t="s">
         <v>35</v>
@@ -2710,8 +3228,29 @@
       <c r="O29" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P29" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q29" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R29" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S29" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T29" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U29" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V29" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="67"/>
       <c r="B30" s="28" t="s">
         <v>35</v>
@@ -2755,8 +3294,29 @@
       <c r="O30" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P30" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q30" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R30" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S30" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T30" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U30" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V30" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="67"/>
       <c r="B31" s="28" t="s">
         <v>35</v>
@@ -2800,8 +3360,29 @@
       <c r="O31" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P31" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q31" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R31" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S31" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T31" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U31" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V31" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="67"/>
       <c r="B32" s="28" t="s">
         <v>35</v>
@@ -2845,8 +3426,29 @@
       <c r="O32" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V32" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="68"/>
       <c r="B33" s="22" t="s">
         <v>35</v>
@@ -2890,8 +3492,29 @@
       <c r="O33" s="30" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P33" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q33" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="R33" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="S33" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="T33" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="U33" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="V33" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="57" t="s">
         <v>41</v>
       </c>
@@ -2937,8 +3560,29 @@
       <c r="O34" s="21">
         <v>48.56</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P34" s="21">
+        <v>49.78</v>
+      </c>
+      <c r="Q34" s="21">
+        <v>50.61</v>
+      </c>
+      <c r="R34" s="21">
+        <v>50.45</v>
+      </c>
+      <c r="S34" s="21">
+        <v>50.61</v>
+      </c>
+      <c r="T34" s="21">
+        <v>49.61</v>
+      </c>
+      <c r="U34" s="21">
+        <v>49.7</v>
+      </c>
+      <c r="V34" s="21">
+        <v>47.95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="58"/>
       <c r="B35" s="18" t="s">
         <v>42</v>
@@ -2982,8 +3626,29 @@
       <c r="O35" s="21">
         <v>43.82</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P35" s="21">
+        <v>44.17</v>
+      </c>
+      <c r="Q35" s="21">
+        <v>45.55</v>
+      </c>
+      <c r="R35" s="21">
+        <v>47.18</v>
+      </c>
+      <c r="S35" s="21">
+        <v>46.88</v>
+      </c>
+      <c r="T35" s="21">
+        <v>47.02</v>
+      </c>
+      <c r="U35" s="21">
+        <v>48.01</v>
+      </c>
+      <c r="V35" s="21">
+        <v>47.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="66" t="s">
         <v>45</v>
       </c>
@@ -3029,8 +3694,29 @@
       <c r="O36" s="17">
         <v>532.98</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P36" s="17">
+        <v>533.24</v>
+      </c>
+      <c r="Q36" s="17">
+        <v>539.55999999999995</v>
+      </c>
+      <c r="R36" s="17">
+        <v>541.23</v>
+      </c>
+      <c r="S36" s="17">
+        <v>541.23</v>
+      </c>
+      <c r="T36" s="17">
+        <v>554.03</v>
+      </c>
+      <c r="U36" s="17">
+        <v>554.03</v>
+      </c>
+      <c r="V36" s="17">
+        <v>549.96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="67"/>
       <c r="B37" s="18" t="s">
         <v>46</v>
@@ -3074,8 +3760,29 @@
       <c r="O37" s="21">
         <v>457.31</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P37" s="21">
+        <v>457.56</v>
+      </c>
+      <c r="Q37" s="21">
+        <v>471.81</v>
+      </c>
+      <c r="R37" s="21">
+        <v>472.73</v>
+      </c>
+      <c r="S37" s="21">
+        <v>472.73</v>
+      </c>
+      <c r="T37" s="21">
+        <v>477.54</v>
+      </c>
+      <c r="U37" s="21">
+        <v>477.64</v>
+      </c>
+      <c r="V37" s="21">
+        <v>471.22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="67"/>
       <c r="B38" s="18" t="s">
         <v>46</v>
@@ -3119,8 +3826,29 @@
       <c r="O38" s="21">
         <v>428.03</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P38" s="21">
+        <v>430.964</v>
+      </c>
+      <c r="Q38" s="21">
+        <v>432.00099999999998</v>
+      </c>
+      <c r="R38" s="21">
+        <v>432.012</v>
+      </c>
+      <c r="S38" s="21">
+        <v>433.83499999999998</v>
+      </c>
+      <c r="T38" s="21">
+        <v>432.72300000000001</v>
+      </c>
+      <c r="U38" s="21">
+        <v>430.17899999999997</v>
+      </c>
+      <c r="V38" s="21">
+        <v>429.31299999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="67"/>
       <c r="B39" s="18" t="s">
         <v>46</v>
@@ -3164,8 +3892,29 @@
       <c r="O39" s="21">
         <v>277.16000000000003</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P39" s="21">
+        <v>282.33999999999997</v>
+      </c>
+      <c r="Q39" s="21">
+        <v>279.93</v>
+      </c>
+      <c r="R39" s="21">
+        <v>279.93</v>
+      </c>
+      <c r="S39" s="21">
+        <v>280.95999999999998</v>
+      </c>
+      <c r="T39" s="21">
+        <v>280.73</v>
+      </c>
+      <c r="U39" s="21">
+        <v>277.83999999999997</v>
+      </c>
+      <c r="V39" s="21">
+        <v>278.95999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="67"/>
       <c r="B40" s="18" t="s">
         <v>14</v>
@@ -3209,8 +3958,29 @@
       <c r="O40" s="21">
         <v>984.88</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P40" s="21">
+        <v>984.88</v>
+      </c>
+      <c r="Q40" s="21">
+        <v>987.3</v>
+      </c>
+      <c r="R40" s="21">
+        <v>987.3</v>
+      </c>
+      <c r="S40" s="21">
+        <v>992.69</v>
+      </c>
+      <c r="T40" s="21">
+        <v>1013.28</v>
+      </c>
+      <c r="U40" s="21">
+        <v>1013.28</v>
+      </c>
+      <c r="V40" s="21">
+        <v>1013.28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="67"/>
       <c r="B41" s="18" t="s">
         <v>14</v>
@@ -3254,8 +4024,29 @@
       <c r="O41" s="21">
         <v>324.02</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P41" s="21">
+        <v>324.02</v>
+      </c>
+      <c r="Q41" s="21">
+        <v>320.33</v>
+      </c>
+      <c r="R41" s="21">
+        <v>320.33</v>
+      </c>
+      <c r="S41" s="21">
+        <v>320.01</v>
+      </c>
+      <c r="T41" s="21">
+        <v>310.17</v>
+      </c>
+      <c r="U41" s="21">
+        <v>302.43</v>
+      </c>
+      <c r="V41" s="21">
+        <v>302.82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="67"/>
       <c r="B42" s="18" t="s">
         <v>14</v>
@@ -3299,8 +4090,29 @@
       <c r="O42" s="21">
         <v>536.57000000000005</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P42" s="21">
+        <v>535.66999999999996</v>
+      </c>
+      <c r="Q42" s="21">
+        <v>554.99</v>
+      </c>
+      <c r="R42" s="21">
+        <v>554.99</v>
+      </c>
+      <c r="S42" s="21">
+        <v>554.99</v>
+      </c>
+      <c r="T42" s="21">
+        <v>555.29</v>
+      </c>
+      <c r="U42" s="21">
+        <v>555.29</v>
+      </c>
+      <c r="V42" s="21">
+        <v>555.29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="67"/>
       <c r="B43" s="18" t="s">
         <v>54</v>
@@ -3344,8 +4156,29 @@
       <c r="O43" s="21">
         <v>193.06</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P43" s="21">
+        <v>190.98</v>
+      </c>
+      <c r="Q43" s="21">
+        <v>191.72900000000001</v>
+      </c>
+      <c r="R43" s="21">
+        <v>193.48</v>
+      </c>
+      <c r="S43" s="21">
+        <v>194.23</v>
+      </c>
+      <c r="T43" s="21">
+        <v>193.82</v>
+      </c>
+      <c r="U43" s="21">
+        <v>196.41200000000001</v>
+      </c>
+      <c r="V43" s="21">
+        <v>203.61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="67"/>
       <c r="B44" s="18" t="s">
         <v>54</v>
@@ -3389,8 +4222,29 @@
       <c r="O44" s="21">
         <v>174.67</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P44" s="21">
+        <v>172.71</v>
+      </c>
+      <c r="Q44" s="21">
+        <v>168.822</v>
+      </c>
+      <c r="R44" s="21">
+        <v>169.47</v>
+      </c>
+      <c r="S44" s="21">
+        <v>169.37</v>
+      </c>
+      <c r="T44" s="21">
+        <v>170.02</v>
+      </c>
+      <c r="U44" s="21">
+        <v>171.86600000000001</v>
+      </c>
+      <c r="V44" s="21">
+        <v>173.88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="67"/>
       <c r="B45" s="18" t="s">
         <v>57</v>
@@ -3434,8 +4288,29 @@
       <c r="O45" s="21">
         <v>207.77099999999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P45" s="21">
+        <v>208.136</v>
+      </c>
+      <c r="Q45" s="21">
+        <v>207.601</v>
+      </c>
+      <c r="R45" s="21">
+        <v>207.66300000000001</v>
+      </c>
+      <c r="S45" s="21">
+        <v>207.66300000000001</v>
+      </c>
+      <c r="T45" s="21">
+        <v>207.66300000000001</v>
+      </c>
+      <c r="U45" s="21">
+        <v>206.92500000000001</v>
+      </c>
+      <c r="V45" s="21">
+        <v>206.822</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="68"/>
       <c r="B46" s="22" t="s">
         <v>57</v>
@@ -3479,8 +4354,29 @@
       <c r="O46" s="25">
         <v>353.714</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P46" s="25">
+        <v>352.73599999999999</v>
+      </c>
+      <c r="Q46" s="25">
+        <v>346.54</v>
+      </c>
+      <c r="R46" s="25">
+        <v>341.36200000000002</v>
+      </c>
+      <c r="S46" s="25">
+        <v>337.52699999999999</v>
+      </c>
+      <c r="T46" s="25">
+        <v>328.09</v>
+      </c>
+      <c r="U46" s="25">
+        <v>326.51799999999997</v>
+      </c>
+      <c r="V46" s="25">
+        <v>326.01400000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="32"/>
       <c r="B47" s="18" t="s">
         <v>60</v>
@@ -3524,8 +4420,29 @@
       <c r="O47" s="21">
         <v>48.423038272931386</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P47" s="21">
+        <v>48.454848723044208</v>
+      </c>
+      <c r="Q47" s="21">
+        <v>51.353373385434864</v>
+      </c>
+      <c r="R47" s="21">
+        <v>51.932477380742995</v>
+      </c>
+      <c r="S47" s="21">
+        <v>50.559931663527571</v>
+      </c>
+      <c r="T47" s="21">
+        <v>50.939973570637385</v>
+      </c>
+      <c r="U47" s="21">
+        <v>52.493012802024026</v>
+      </c>
+      <c r="V47" s="21">
+        <v>54.702060714305333</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="33"/>
       <c r="B48" s="18" t="s">
         <v>60</v>
@@ -3569,8 +4486,29 @@
       <c r="O48" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P48" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q48" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R48" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S48" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T48" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U48" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V48" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="33"/>
       <c r="B49" s="18" t="s">
         <v>60</v>
@@ -3614,8 +4552,29 @@
       <c r="O49" s="21">
         <v>85.794365131564021</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P49" s="21">
+        <v>101.47854602964368</v>
+      </c>
+      <c r="Q49" s="21">
+        <v>99.617824639943464</v>
+      </c>
+      <c r="R49" s="21">
+        <v>102.95702883397639</v>
+      </c>
+      <c r="S49" s="21">
+        <v>90</v>
+      </c>
+      <c r="T49" s="21">
+        <v>91</v>
+      </c>
+      <c r="U49" s="21">
+        <v>84.748500000000007</v>
+      </c>
+      <c r="V49" s="21">
+        <v>78.624250000000018</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="33"/>
       <c r="B50" s="18" t="s">
         <v>60</v>
@@ -3659,8 +4618,29 @@
       <c r="O50" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P50" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q50" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R50" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S50" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T50" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U50" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V50" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="33"/>
       <c r="B51" s="18" t="s">
         <v>60</v>
@@ -3704,8 +4684,29 @@
       <c r="O51" s="21">
         <v>35.15080091830972</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P51" s="21">
+        <v>36.179126889806952</v>
+      </c>
+      <c r="Q51" s="21">
+        <v>37.006983337794381</v>
+      </c>
+      <c r="R51" s="21">
+        <v>39.009157791723659</v>
+      </c>
+      <c r="S51" s="21">
+        <v>40.830253457856784</v>
+      </c>
+      <c r="T51" s="21">
+        <v>41.690007557111187</v>
+      </c>
+      <c r="U51" s="21">
+        <v>43.277019652622023</v>
+      </c>
+      <c r="V51" s="21">
+        <v>43.721710465689938</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="33"/>
       <c r="B52" s="18" t="s">
         <v>60</v>
@@ -3749,8 +4750,29 @@
       <c r="O52" s="21">
         <v>36.483928710035144</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P52" s="21">
+        <v>36.900403311179168</v>
+      </c>
+      <c r="Q52" s="21">
+        <v>37.504523813730728</v>
+      </c>
+      <c r="R52" s="21">
+        <v>39.134767821652055</v>
+      </c>
+      <c r="S52" s="21">
+        <v>40.927369013392784</v>
+      </c>
+      <c r="T52" s="21">
+        <v>40.274555039764302</v>
+      </c>
+      <c r="U52" s="21">
+        <v>42.411929053059907</v>
+      </c>
+      <c r="V52" s="21">
+        <v>44.74598415617865</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="33"/>
       <c r="B53" s="18" t="s">
         <v>60</v>
@@ -3794,8 +4816,29 @@
       <c r="O53" s="21">
         <v>33.225364100152326</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P53" s="21">
+        <v>32.58716251771915</v>
+      </c>
+      <c r="Q53" s="21">
+        <v>33.020506246450282</v>
+      </c>
+      <c r="R53" s="21">
+        <v>33.378755256706867</v>
+      </c>
+      <c r="S53" s="21">
+        <v>35.133595840950385</v>
+      </c>
+      <c r="T53" s="21">
+        <v>32.049103654489869</v>
+      </c>
+      <c r="U53" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V53" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="33"/>
       <c r="B54" s="18" t="s">
         <v>60</v>
@@ -3839,8 +4882,29 @@
       <c r="O54" s="21">
         <v>38.92106373934827</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P54" s="21">
+        <v>38.397856010262778</v>
+      </c>
+      <c r="Q54" s="21">
+        <v>39</v>
+      </c>
+      <c r="R54" s="21">
+        <v>41.607647009838949</v>
+      </c>
+      <c r="S54" s="21">
+        <v>40.350532281520813</v>
+      </c>
+      <c r="T54" s="21">
+        <v>40.364750839931681</v>
+      </c>
+      <c r="U54" s="21">
+        <v>40.967635677413263</v>
+      </c>
+      <c r="V54" s="21">
+        <v>41.397695978485828</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="33"/>
       <c r="B55" s="18" t="s">
         <v>60</v>
@@ -3884,8 +4948,29 @@
       <c r="O55" s="21">
         <v>31.592911325207265</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P55" s="21">
+        <v>30</v>
+      </c>
+      <c r="Q55" s="21">
+        <v>30.999999999999996</v>
+      </c>
+      <c r="R55" s="21">
+        <v>32</v>
+      </c>
+      <c r="S55" s="21">
+        <v>31.000000000000004</v>
+      </c>
+      <c r="T55" s="21">
+        <v>31.000000000000004</v>
+      </c>
+      <c r="U55" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V55" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="33"/>
       <c r="B56" s="18" t="s">
         <v>60</v>
@@ -3929,8 +5014,29 @@
       <c r="O56" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P56" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q56" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R56" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S56" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T56" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U56" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V56" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="33"/>
       <c r="B57" s="18" t="s">
         <v>60</v>
@@ -3974,8 +5080,29 @@
       <c r="O57" s="21">
         <v>30.231859460564529</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P57" s="21">
+        <v>33.517779257866934</v>
+      </c>
+      <c r="Q57" s="21">
+        <v>36.373723604956922</v>
+      </c>
+      <c r="R57" s="21">
+        <v>38.849283815954209</v>
+      </c>
+      <c r="S57" s="21">
+        <v>40.706646688704275</v>
+      </c>
+      <c r="T57" s="21">
+        <v>43.491567684038216</v>
+      </c>
+      <c r="U57" s="21">
+        <v>43.461818617046958</v>
+      </c>
+      <c r="V57" s="21">
+        <v>43.502907120253248</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="33"/>
       <c r="B58" s="18" t="s">
         <v>60</v>
@@ -4019,8 +5146,29 @@
       <c r="O58" s="21">
         <v>21.626398819555313</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P58" s="21">
+        <v>21.25</v>
+      </c>
+      <c r="Q58" s="21">
+        <v>22</v>
+      </c>
+      <c r="R58" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S58" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T58" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U58" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V58" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A59" s="33"/>
       <c r="B59" s="18" t="s">
         <v>60</v>
@@ -4064,8 +5212,29 @@
       <c r="O59" s="21">
         <v>33.025358029328189</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P59" s="21">
+        <v>34.490100781649737</v>
+      </c>
+      <c r="Q59" s="21">
+        <v>36.720284020839557</v>
+      </c>
+      <c r="R59" s="21">
+        <v>37.282077984574933</v>
+      </c>
+      <c r="S59" s="21">
+        <v>39.697489879169659</v>
+      </c>
+      <c r="T59" s="21">
+        <v>41.441214424494355</v>
+      </c>
+      <c r="U59" s="21">
+        <v>41.215991470807964</v>
+      </c>
+      <c r="V59" s="21">
+        <v>41.073338870310067</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="33"/>
       <c r="B60" s="18" t="s">
         <v>73</v>
@@ -4109,8 +5278,29 @@
       <c r="O60" s="21">
         <v>58.601082250162079</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P60" s="21">
+        <v>58.984961017981078</v>
+      </c>
+      <c r="Q60" s="21">
+        <v>59.805420091668914</v>
+      </c>
+      <c r="R60" s="21">
+        <v>59.114600873550827</v>
+      </c>
+      <c r="S60" s="21">
+        <v>59.710276645996224</v>
+      </c>
+      <c r="T60" s="21">
+        <v>60.831489781612298</v>
+      </c>
+      <c r="U60" s="21">
+        <v>64.168321827438078</v>
+      </c>
+      <c r="V60" s="21">
+        <v>66.864391168192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="33"/>
       <c r="B61" s="18" t="s">
         <v>73</v>
@@ -4154,8 +5344,29 @@
       <c r="O61" s="21">
         <v>69.498932391523724</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P61" s="21">
+        <v>69.505272653884973</v>
+      </c>
+      <c r="Q61" s="21">
+        <v>69.734459430436843</v>
+      </c>
+      <c r="R61" s="21">
+        <v>69.681051930758983</v>
+      </c>
+      <c r="S61" s="21">
+        <v>69.732575490743528</v>
+      </c>
+      <c r="T61" s="21">
+        <v>74.396053863665642</v>
+      </c>
+      <c r="U61" s="21">
+        <v>78.1649113869465</v>
+      </c>
+      <c r="V61" s="21">
+        <v>81.980700848506828</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A62" s="33"/>
       <c r="B62" s="18" t="s">
         <v>73</v>
@@ -4199,8 +5410,29 @@
       <c r="O62" s="21">
         <v>74.812917251051886</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P62" s="21">
+        <v>69.381935483870961</v>
+      </c>
+      <c r="Q62" s="21">
+        <v>72.285175315568011</v>
+      </c>
+      <c r="R62" s="21">
+        <v>64.412528050490877</v>
+      </c>
+      <c r="S62" s="21">
+        <v>57.443816619915843</v>
+      </c>
+      <c r="T62" s="21">
+        <v>51.665708274894804</v>
+      </c>
+      <c r="U62" s="21">
+        <v>52.028021978021982</v>
+      </c>
+      <c r="V62" s="21">
+        <v>51.444986263736261</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="33"/>
       <c r="B63" s="18" t="s">
         <v>73</v>
@@ -4244,8 +5476,29 @@
       <c r="O63" s="21">
         <v>62.093800000000002</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P63" s="21">
+        <v>64.610266026602659</v>
+      </c>
+      <c r="Q63" s="21">
+        <v>64.02944794479447</v>
+      </c>
+      <c r="R63" s="21">
+        <v>62.028487848784884</v>
+      </c>
+      <c r="S63" s="21">
+        <v>64.047376737673758</v>
+      </c>
+      <c r="T63" s="21">
+        <v>61.237879787978798</v>
+      </c>
+      <c r="U63" s="21">
+        <v>68.846603962377429</v>
+      </c>
+      <c r="V63" s="21">
+        <v>68.992404399999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="34" t="s">
         <v>78</v>
       </c>
@@ -4291,8 +5544,29 @@
       <c r="O64" s="21">
         <v>76.450393039303918</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P64" s="21">
+        <v>80.12556255625563</v>
+      </c>
+      <c r="Q64" s="21">
+        <v>79.75043804380438</v>
+      </c>
+      <c r="R64" s="21">
+        <v>73.277472747274714</v>
+      </c>
+      <c r="S64" s="21">
+        <v>78.931518151815183</v>
+      </c>
+      <c r="T64" s="21">
+        <v>77.834861486148611</v>
+      </c>
+      <c r="U64" s="21">
+        <v>74.772812281228127</v>
+      </c>
+      <c r="V64" s="21">
+        <v>76.580922599999994</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A65" s="35"/>
       <c r="B65" s="18" t="s">
         <v>73</v>
@@ -4336,8 +5610,29 @@
       <c r="O65" s="21">
         <v>127.95999999999998</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P65" s="21">
+        <v>138.18</v>
+      </c>
+      <c r="Q65" s="21">
+        <v>148.06</v>
+      </c>
+      <c r="R65" s="21">
+        <v>148.72</v>
+      </c>
+      <c r="S65" s="21">
+        <v>148.72</v>
+      </c>
+      <c r="T65" s="21">
+        <v>153.72</v>
+      </c>
+      <c r="U65" s="21">
+        <v>154.24</v>
+      </c>
+      <c r="V65" s="21">
+        <v>157.56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A66" s="33"/>
       <c r="B66" s="18" t="s">
         <v>73</v>
@@ -4381,8 +5676,29 @@
       <c r="O66" s="21">
         <v>83.612618781208752</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P66" s="21">
+        <v>83.612618781208752</v>
+      </c>
+      <c r="Q66" s="21">
+        <v>84.166291023514532</v>
+      </c>
+      <c r="R66" s="21">
+        <v>84.166291023514532</v>
+      </c>
+      <c r="S66" s="21">
+        <v>84.166291023514532</v>
+      </c>
+      <c r="T66" s="21">
+        <v>83.483021658927697</v>
+      </c>
+      <c r="U66" s="21">
+        <v>82.86047157582864</v>
+      </c>
+      <c r="V66" s="21">
+        <v>82.86047157582864</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A67" s="33"/>
       <c r="B67" s="18" t="s">
         <v>73</v>
@@ -4426,8 +5742,29 @@
       <c r="O67" s="21">
         <v>89.425137425213364</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P67" s="21">
+        <v>89.425137425213364</v>
+      </c>
+      <c r="Q67" s="21">
+        <v>89.142048588013893</v>
+      </c>
+      <c r="R67" s="21">
+        <v>94.298541108780057</v>
+      </c>
+      <c r="S67" s="21">
+        <v>94.298541108780057</v>
+      </c>
+      <c r="T67" s="21">
+        <v>94.788003092894854</v>
+      </c>
+      <c r="U67" s="21">
+        <v>90.745095982900125</v>
+      </c>
+      <c r="V67" s="21">
+        <v>88.235663465650632</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A68" s="33"/>
       <c r="B68" s="36" t="s">
         <v>73</v>
@@ -4471,8 +5808,29 @@
       <c r="O68" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P68" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q68" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R68" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S68" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T68" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U68" s="21">
+        <v>107.5</v>
+      </c>
+      <c r="V68" s="21">
+        <v>164.76946004568813</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A69" s="33"/>
       <c r="B69" s="36" t="s">
         <v>73</v>
@@ -4516,8 +5874,29 @@
       <c r="O69" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P69" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q69" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R69" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S69" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T69" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U69" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V69" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A70" s="33"/>
       <c r="B70" s="36" t="s">
         <v>73</v>
@@ -4561,8 +5940,29 @@
       <c r="O70" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P70" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q70" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R70" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S70" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T70" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U70" s="21">
+        <v>107.5</v>
+      </c>
+      <c r="V70" s="21">
+        <v>204.64913306286613</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A71" s="33"/>
       <c r="B71" s="36" t="s">
         <v>73</v>
@@ -4606,8 +6006,29 @@
       <c r="O71" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P71" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q71" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R71" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S71" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T71" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U71" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V71" s="21">
+        <v>173.81660362271086</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A72" s="33"/>
       <c r="B72" s="36" t="s">
         <v>73</v>
@@ -4651,8 +6072,29 @@
       <c r="O72" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P72" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q72" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R72" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S72" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T72" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U72" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V72" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A73" s="35"/>
       <c r="B73" s="36" t="s">
         <v>73</v>
@@ -4696,8 +6138,29 @@
       <c r="O73" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P73" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q73" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R73" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S73" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T73" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U73" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V73" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A74" s="33"/>
       <c r="B74" s="36" t="s">
         <v>73</v>
@@ -4741,8 +6204,29 @@
       <c r="O74" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P74" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q74" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R74" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S74" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T74" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U74" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V74" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A75" s="33"/>
       <c r="B75" s="36" t="s">
         <v>73</v>
@@ -4786,8 +6270,29 @@
       <c r="O75" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P75" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q75" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R75" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S75" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T75" s="21">
+        <v>94</v>
+      </c>
+      <c r="U75" s="21">
+        <v>84</v>
+      </c>
+      <c r="V75" s="21">
+        <v>80.666666666666671</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" s="33"/>
       <c r="B76" s="36" t="s">
         <v>73</v>
@@ -4831,8 +6336,29 @@
       <c r="O76" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P76" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q76" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R76" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S76" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T76" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U76" s="21">
+        <v>610</v>
+      </c>
+      <c r="V76" s="21">
+        <v>389.52207995085814</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A77" s="33"/>
       <c r="B77" s="36" t="s">
         <v>73</v>
@@ -4876,8 +6402,29 @@
       <c r="O77" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P77" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q77" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R77" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S77" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T77" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U77" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V77" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A78" s="33"/>
       <c r="B78" s="36" t="s">
         <v>73</v>
@@ -4921,8 +6468,29 @@
       <c r="O78" s="21">
         <v>242.14441786207416</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P78" s="21">
+        <v>260.61733123657558</v>
+      </c>
+      <c r="Q78" s="21">
+        <v>252.55288944812017</v>
+      </c>
+      <c r="R78" s="21">
+        <v>264.37073300455506</v>
+      </c>
+      <c r="S78" s="21">
+        <v>268.87952042930198</v>
+      </c>
+      <c r="T78" s="21">
+        <v>269.47281535917614</v>
+      </c>
+      <c r="U78" s="21">
+        <v>255.92</v>
+      </c>
+      <c r="V78" s="21">
+        <v>311.72000000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A79" s="33"/>
       <c r="B79" s="36" t="s">
         <v>73</v>
@@ -4957,17 +6525,38 @@
       <c r="L79" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="M79" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="N79" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="O79" s="21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M79" s="21">
+        <v>236</v>
+      </c>
+      <c r="N79" s="21">
+        <v>268</v>
+      </c>
+      <c r="O79" s="21">
+        <v>295</v>
+      </c>
+      <c r="P79" s="21">
+        <v>240</v>
+      </c>
+      <c r="Q79" s="21">
+        <v>241.10582117155886</v>
+      </c>
+      <c r="R79" s="21">
+        <v>210.21735547783413</v>
+      </c>
+      <c r="S79" s="21">
+        <v>184.54719745106294</v>
+      </c>
+      <c r="T79" s="21">
+        <v>144.875135046053</v>
+      </c>
+      <c r="U79" s="21">
+        <v>155.93144722259285</v>
+      </c>
+      <c r="V79" s="21">
+        <v>170.76240378102557</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A80" s="33"/>
       <c r="B80" s="36" t="s">
         <v>73</v>
@@ -5011,8 +6600,29 @@
       <c r="O80" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P80" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q80" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R80" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S80" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T80" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U80" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V80" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A81" s="33"/>
       <c r="B81" s="36" t="s">
         <v>73</v>
@@ -5056,8 +6666,29 @@
       <c r="O81" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P81" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q81" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R81" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S81" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T81" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U81" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V81" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A82" s="33"/>
       <c r="B82" s="36" t="s">
         <v>73</v>
@@ -5101,8 +6732,29 @@
       <c r="O82" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P82" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q82" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R82" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S82" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T82" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U82" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V82" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A83" s="38"/>
       <c r="B83" s="39" t="s">
         <v>73</v>
@@ -5146,8 +6798,29 @@
       <c r="O83" s="25" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P83" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q83" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="R83" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="S83" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="T83" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="U83" s="25">
+        <v>154.99999999999997</v>
+      </c>
+      <c r="V83" s="25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="84" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A84" s="41"/>
       <c r="B84" s="18" t="s">
         <v>73</v>
@@ -5191,8 +6864,29 @@
       <c r="O84" s="21">
         <v>33.777008484784908</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P84" s="21">
+        <v>34.260058688016905</v>
+      </c>
+      <c r="Q84" s="21">
+        <v>33.318878374000299</v>
+      </c>
+      <c r="R84" s="21">
+        <v>35.543083006492765</v>
+      </c>
+      <c r="S84" s="21">
+        <v>33.693060101376986</v>
+      </c>
+      <c r="T84" s="21">
+        <v>32.357086222915953</v>
+      </c>
+      <c r="U84" s="21">
+        <v>33.006628984480393</v>
+      </c>
+      <c r="V84" s="21">
+        <v>35.118380661114045</v>
+      </c>
+    </row>
+    <row r="85" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A85" s="42"/>
       <c r="B85" s="18" t="s">
         <v>73</v>
@@ -5236,8 +6930,29 @@
       <c r="O85" s="21">
         <v>49.599008699776093</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P85" s="21">
+        <v>47.028241813347435</v>
+      </c>
+      <c r="Q85" s="21">
+        <v>51.506265067551553</v>
+      </c>
+      <c r="R85" s="21">
+        <v>51.708113738483185</v>
+      </c>
+      <c r="S85" s="21">
+        <v>57.966532474016248</v>
+      </c>
+      <c r="T85" s="21">
+        <v>62.972943312304267</v>
+      </c>
+      <c r="U85" s="21">
+        <v>67.7533074509263</v>
+      </c>
+      <c r="V85" s="21">
+        <v>63.777972882539501</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A86" s="42"/>
       <c r="B86" s="18" t="s">
         <v>73</v>
@@ -5281,8 +6996,29 @@
       <c r="O86" s="21">
         <v>92.371006897688005</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P86" s="21">
+        <v>93.107063904211842</v>
+      </c>
+      <c r="Q86" s="21">
+        <v>101.47261166225255</v>
+      </c>
+      <c r="R86" s="21">
+        <v>98.677020129900058</v>
+      </c>
+      <c r="S86" s="21">
+        <v>105.43142379069064</v>
+      </c>
+      <c r="T86" s="21">
+        <v>103.36872832369944</v>
+      </c>
+      <c r="U86" s="21">
+        <v>107.30888730662183</v>
+      </c>
+      <c r="V86" s="21">
+        <v>107.30888730662183</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A87" s="42"/>
       <c r="B87" s="18" t="s">
         <v>73</v>
@@ -5326,8 +7062,29 @@
       <c r="O87" s="21">
         <v>93.63229221738851</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P87" s="21">
+        <v>75.396496722871845</v>
+      </c>
+      <c r="Q87" s="21">
+        <v>74.614700954823462</v>
+      </c>
+      <c r="R87" s="21">
+        <v>75.933040810866288</v>
+      </c>
+      <c r="S87" s="21">
+        <v>65.061349313922776</v>
+      </c>
+      <c r="T87" s="21">
+        <v>46.733886114621484</v>
+      </c>
+      <c r="U87" s="21">
+        <v>66.658486163478671</v>
+      </c>
+      <c r="V87" s="21">
+        <v>56.563801661596507</v>
+      </c>
+    </row>
+    <row r="88" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A88" s="42"/>
       <c r="B88" s="18" t="s">
         <v>73</v>
@@ -5371,8 +7128,29 @@
       <c r="O88" s="21">
         <v>154.43170293727525</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P88" s="21">
+        <v>155.97401325189836</v>
+      </c>
+      <c r="Q88" s="21">
+        <v>155.65971695632993</v>
+      </c>
+      <c r="R88" s="21">
+        <v>153.91178662410141</v>
+      </c>
+      <c r="S88" s="21">
+        <v>156.27518760124377</v>
+      </c>
+      <c r="T88" s="21">
+        <v>140.97535451189938</v>
+      </c>
+      <c r="U88" s="21">
+        <v>115.14792061938542</v>
+      </c>
+      <c r="V88" s="21">
+        <v>104.08652528782346</v>
+      </c>
+    </row>
+    <row r="89" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A89" s="42"/>
       <c r="B89" s="18" t="s">
         <v>73</v>
@@ -5416,8 +7194,29 @@
       <c r="O89" s="21">
         <v>106.85674453779053</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P89" s="21">
+        <v>84.639685091408595</v>
+      </c>
+      <c r="Q89" s="21">
+        <v>92.571781702351018</v>
+      </c>
+      <c r="R89" s="21">
+        <v>82.292693775609678</v>
+      </c>
+      <c r="S89" s="21">
+        <v>51.603859011656219</v>
+      </c>
+      <c r="T89" s="21">
+        <v>51.603859011656219</v>
+      </c>
+      <c r="U89" s="21">
+        <v>34.5</v>
+      </c>
+      <c r="V89" s="21">
+        <v>21.956758500000003</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A90" s="42"/>
       <c r="B90" s="18" t="s">
         <v>73</v>
@@ -5461,8 +7260,29 @@
       <c r="O90" s="21">
         <v>125.96010202141913</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P90" s="21">
+        <v>115.40713888651169</v>
+      </c>
+      <c r="Q90" s="21">
+        <v>106.85537683042631</v>
+      </c>
+      <c r="R90" s="21">
+        <v>102.26143518144325</v>
+      </c>
+      <c r="S90" s="21">
+        <v>90.176815980283308</v>
+      </c>
+      <c r="T90" s="21">
+        <v>82.385805511377271</v>
+      </c>
+      <c r="U90" s="21">
+        <v>71.740387941012912</v>
+      </c>
+      <c r="V90" s="21">
+        <v>60.42524906589955</v>
+      </c>
+    </row>
+    <row r="91" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A91" s="42"/>
       <c r="B91" s="18" t="s">
         <v>73</v>
@@ -5506,8 +7326,29 @@
       <c r="O91" s="21">
         <v>68.668561751710868</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P91" s="21">
+        <v>73.535986074081734</v>
+      </c>
+      <c r="Q91" s="21">
+        <v>70.587004563969543</v>
+      </c>
+      <c r="R91" s="21">
+        <v>56.368000072942792</v>
+      </c>
+      <c r="S91" s="21">
+        <v>49.649536493188776</v>
+      </c>
+      <c r="T91" s="21">
+        <v>45.073116947652004</v>
+      </c>
+      <c r="U91" s="21">
+        <v>45.24259441087176</v>
+      </c>
+      <c r="V91" s="21">
+        <v>47.287513970611606</v>
+      </c>
+    </row>
+    <row r="92" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A92" s="42"/>
       <c r="B92" s="18" t="s">
         <v>73</v>
@@ -5551,8 +7392,29 @@
       <c r="O92" s="21">
         <v>78.370309419517255</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P92" s="21">
+        <v>83.808875409297229</v>
+      </c>
+      <c r="Q92" s="21">
+        <v>88.006428594316887</v>
+      </c>
+      <c r="R92" s="21">
+        <v>73.782416429405558</v>
+      </c>
+      <c r="S92" s="21">
+        <v>88.586516230776553</v>
+      </c>
+      <c r="T92" s="21">
+        <v>81.563061920738903</v>
+      </c>
+      <c r="U92" s="21">
+        <v>71.416800416807689</v>
+      </c>
+      <c r="V92" s="21">
+        <v>57.202501454212239</v>
+      </c>
+    </row>
+    <row r="93" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A93" s="42"/>
       <c r="B93" s="18" t="s">
         <v>73</v>
@@ -5596,8 +7458,29 @@
       <c r="O93" s="21">
         <v>67.898519930692188</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P93" s="21">
+        <v>99.19991500871042</v>
+      </c>
+      <c r="Q93" s="21">
+        <v>81.255059948654903</v>
+      </c>
+      <c r="R93" s="21">
+        <v>55.710418344191012</v>
+      </c>
+      <c r="S93" s="21">
+        <v>44.553843365663752</v>
+      </c>
+      <c r="T93" s="21">
+        <v>39.277951756264336</v>
+      </c>
+      <c r="U93" s="21">
+        <v>38.172195498811618</v>
+      </c>
+      <c r="V93" s="21">
+        <v>41.1531377431686</v>
+      </c>
+    </row>
+    <row r="94" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A94" s="42"/>
       <c r="B94" s="18" t="s">
         <v>73</v>
@@ -5641,8 +7524,29 @@
       <c r="O94" s="21">
         <v>63.301286614932067</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P94" s="21">
+        <v>40.245038294926893</v>
+      </c>
+      <c r="Q94" s="21">
+        <v>46.56763229007916</v>
+      </c>
+      <c r="R94" s="21">
+        <v>53.243765608464138</v>
+      </c>
+      <c r="S94" s="21">
+        <v>51.847803396731749</v>
+      </c>
+      <c r="T94" s="21">
+        <v>43.398841856022116</v>
+      </c>
+      <c r="U94" s="21">
+        <v>28.509063929205791</v>
+      </c>
+      <c r="V94" s="21">
+        <v>28.204408001522363</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A95" s="42"/>
       <c r="B95" s="18" t="s">
         <v>73</v>
@@ -5686,8 +7590,29 @@
       <c r="O95" s="21">
         <v>151.56621846208111</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P95" s="21">
+        <v>142.68351160017875</v>
+      </c>
+      <c r="Q95" s="21">
+        <v>149.63565897251996</v>
+      </c>
+      <c r="R95" s="21">
+        <v>145.79752003331035</v>
+      </c>
+      <c r="S95" s="21">
+        <v>139.57212795305514</v>
+      </c>
+      <c r="T95" s="21">
+        <v>119.45914738718481</v>
+      </c>
+      <c r="U95" s="21">
+        <v>91.797032470476879</v>
+      </c>
+      <c r="V95" s="21">
+        <v>73.995346365295504</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="43" t="s">
         <v>111</v>
       </c>
@@ -5733,8 +7658,29 @@
       <c r="O96" s="21">
         <v>31.471742382530319</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P96" s="21">
+        <v>35.703935524820707</v>
+      </c>
+      <c r="Q96" s="21">
+        <v>41.858669159817666</v>
+      </c>
+      <c r="R96" s="21">
+        <v>47.519749247443379</v>
+      </c>
+      <c r="S96" s="21">
+        <v>56.315388703026677</v>
+      </c>
+      <c r="T96" s="21">
+        <v>51.760792224153761</v>
+      </c>
+      <c r="U96" s="21">
+        <v>49.202941522184204</v>
+      </c>
+      <c r="V96" s="21">
+        <v>51.220968912857174</v>
+      </c>
+    </row>
+    <row r="97" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A97" s="42"/>
       <c r="B97" s="18" t="s">
         <v>73</v>
@@ -5778,8 +7724,29 @@
       <c r="O97" s="21">
         <v>187.71571064957556</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P97" s="21">
+        <v>187.67172555399571</v>
+      </c>
+      <c r="Q97" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R97" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S97" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T97" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U97" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V97" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="98" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A98" s="42"/>
       <c r="B98" s="18" t="s">
         <v>73</v>
@@ -5823,8 +7790,29 @@
       <c r="O98" s="21">
         <v>39.74230616386685</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P98" s="21">
+        <v>33.052667285431717</v>
+      </c>
+      <c r="Q98" s="21">
+        <v>27.713552562212335</v>
+      </c>
+      <c r="R98" s="21">
+        <v>23.400681975237188</v>
+      </c>
+      <c r="S98" s="21">
+        <v>19.907410309393544</v>
+      </c>
+      <c r="T98" s="21">
+        <v>20.50794840297451</v>
+      </c>
+      <c r="U98" s="21">
+        <v>14.903106783122039</v>
+      </c>
+      <c r="V98" s="21">
+        <v>15.441205016927137</v>
+      </c>
+    </row>
+    <row r="99" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A99" s="42"/>
       <c r="B99" s="18" t="s">
         <v>73</v>
@@ -5868,8 +7856,29 @@
       <c r="O99" s="21">
         <v>319.39761076326056</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P99" s="21">
+        <v>281.52082317055175</v>
+      </c>
+      <c r="Q99" s="21">
+        <v>203.42760127678255</v>
+      </c>
+      <c r="R99" s="21">
+        <v>184.8663729582384</v>
+      </c>
+      <c r="S99" s="21">
+        <v>145.35308859234868</v>
+      </c>
+      <c r="T99" s="21">
+        <v>132.57418693874624</v>
+      </c>
+      <c r="U99" s="21">
+        <v>135.65112680124386</v>
+      </c>
+      <c r="V99" s="21">
+        <v>116.01356294881904</v>
+      </c>
+    </row>
+    <row r="100" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A100" s="42"/>
       <c r="B100" s="18" t="s">
         <v>73</v>
@@ -5913,8 +7922,29 @@
       <c r="O100" s="21">
         <v>71.025901273607971</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P100" s="21">
+        <v>67.876526018182929</v>
+      </c>
+      <c r="Q100" s="21">
+        <v>67.084311224489795</v>
+      </c>
+      <c r="R100" s="21">
+        <v>69.616953022456897</v>
+      </c>
+      <c r="S100" s="21">
+        <v>66.532087464073641</v>
+      </c>
+      <c r="T100" s="21">
+        <v>65.545086370983739</v>
+      </c>
+      <c r="U100" s="21">
+        <v>68.724112049487431</v>
+      </c>
+      <c r="V100" s="21">
+        <v>74.070157120107453</v>
+      </c>
+    </row>
+    <row r="101" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A101" s="42"/>
       <c r="B101" s="18" t="s">
         <v>73</v>
@@ -5958,8 +7988,29 @@
       <c r="O101" s="21">
         <v>35.911117528154776</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P101" s="21">
+        <v>39.519645056760737</v>
+      </c>
+      <c r="Q101" s="21">
+        <v>42.93864768959299</v>
+      </c>
+      <c r="R101" s="21">
+        <v>40.851500654934789</v>
+      </c>
+      <c r="S101" s="21">
+        <v>40.851500654934789</v>
+      </c>
+      <c r="T101" s="21">
+        <v>39.394256506634768</v>
+      </c>
+      <c r="U101" s="21">
+        <v>40.163066253518288</v>
+      </c>
+      <c r="V101" s="21">
+        <v>38.872299690138711</v>
+      </c>
+    </row>
+    <row r="102" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A102" s="42"/>
       <c r="B102" s="18" t="s">
         <v>73</v>
@@ -6003,8 +8054,29 @@
       <c r="O102" s="21">
         <v>246.06610524693173</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P102" s="21">
+        <v>196.29224748957662</v>
+      </c>
+      <c r="Q102" s="21">
+        <v>114.75870053217814</v>
+      </c>
+      <c r="R102" s="21">
+        <v>118.35860814947424</v>
+      </c>
+      <c r="S102" s="21">
+        <v>124.96294075164816</v>
+      </c>
+      <c r="T102" s="21">
+        <v>164.79082727733757</v>
+      </c>
+      <c r="U102" s="21">
+        <v>166.92910805476976</v>
+      </c>
+      <c r="V102" s="21">
+        <v>217.69120470577451</v>
+      </c>
+    </row>
+    <row r="103" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A103" s="42"/>
       <c r="B103" s="18" t="s">
         <v>73</v>
@@ -6048,8 +8120,29 @@
       <c r="O103" s="21">
         <v>36.308575131054802</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P103" s="21">
+        <v>24.052750572325586</v>
+      </c>
+      <c r="Q103" s="21">
+        <v>16.965577447379459</v>
+      </c>
+      <c r="R103" s="21">
+        <v>34.158983030300242</v>
+      </c>
+      <c r="S103" s="21">
+        <v>56.196416407058102</v>
+      </c>
+      <c r="T103" s="21">
+        <v>41.287846795360842</v>
+      </c>
+      <c r="U103" s="21">
+        <v>34.658060552233103</v>
+      </c>
+      <c r="V103" s="21">
+        <v>34.722529045842826</v>
+      </c>
+    </row>
+    <row r="104" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A104" s="42"/>
       <c r="B104" s="18" t="s">
         <v>73</v>
@@ -6093,8 +8186,29 @@
       <c r="O104" s="21">
         <v>290.4033527137637</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P104" s="21">
+        <v>328.04766579835899</v>
+      </c>
+      <c r="Q104" s="21">
+        <v>306.11142866769779</v>
+      </c>
+      <c r="R104" s="21">
+        <v>282.70595774739024</v>
+      </c>
+      <c r="S104" s="21">
+        <v>280.7969339741685</v>
+      </c>
+      <c r="T104" s="21">
+        <v>275.61866740499005</v>
+      </c>
+      <c r="U104" s="21">
+        <v>249.55688026628428</v>
+      </c>
+      <c r="V104" s="21">
+        <v>258.39077960594631</v>
+      </c>
+    </row>
+    <row r="105" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A105" s="42"/>
       <c r="B105" s="18" t="s">
         <v>73</v>
@@ -6138,8 +8252,29 @@
       <c r="O105" s="21">
         <v>132.4622542023188</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P105" s="21">
+        <v>143.00463404941462</v>
+      </c>
+      <c r="Q105" s="21">
+        <v>117.57154139479704</v>
+      </c>
+      <c r="R105" s="21">
+        <v>93.920771686015286</v>
+      </c>
+      <c r="S105" s="21">
+        <v>77.929561901533759</v>
+      </c>
+      <c r="T105" s="21">
+        <v>78.394697624495095</v>
+      </c>
+      <c r="U105" s="21">
+        <v>72.355644376120921</v>
+      </c>
+      <c r="V105" s="21">
+        <v>67.666226266919224</v>
+      </c>
+    </row>
+    <row r="106" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A106" s="42"/>
       <c r="B106" s="18" t="s">
         <v>73</v>
@@ -6183,8 +8318,29 @@
       <c r="O106" s="21">
         <v>70.143926505614161</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P106" s="21">
+        <v>72.438584552568898</v>
+      </c>
+      <c r="Q106" s="21">
+        <v>78.650782259222055</v>
+      </c>
+      <c r="R106" s="21">
+        <v>78.61039696321123</v>
+      </c>
+      <c r="S106" s="21">
+        <v>77.29480598952297</v>
+      </c>
+      <c r="T106" s="21">
+        <v>76.097364980761213</v>
+      </c>
+      <c r="U106" s="21">
+        <v>80.436213991769534</v>
+      </c>
+      <c r="V106" s="21">
+        <v>77.186634309665251</v>
+      </c>
+    </row>
+    <row r="107" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A107" s="42"/>
       <c r="B107" s="18" t="s">
         <v>73</v>
@@ -6228,8 +8384,29 @@
       <c r="O107" s="21">
         <v>204.69351367201642</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P107" s="21">
+        <v>203.81140681560748</v>
+      </c>
+      <c r="Q107" s="21">
+        <v>209.74459463951871</v>
+      </c>
+      <c r="R107" s="21">
+        <v>215.74977776029399</v>
+      </c>
+      <c r="S107" s="21">
+        <v>216.37743981146318</v>
+      </c>
+      <c r="T107" s="21">
+        <v>215.9711478719023</v>
+      </c>
+      <c r="U107" s="21">
+        <v>214.16605590185279</v>
+      </c>
+      <c r="V107" s="21">
+        <v>214.95577954851547</v>
+      </c>
+    </row>
+    <row r="108" spans="1:22" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A108" s="44"/>
       <c r="B108" s="18" t="s">
         <v>73</v>
@@ -6273,8 +8450,29 @@
       <c r="O108" s="21">
         <v>69.39299281553906</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P108" s="21">
+        <v>70.636812325490354</v>
+      </c>
+      <c r="Q108" s="21">
+        <v>75.863107029224011</v>
+      </c>
+      <c r="R108" s="21">
+        <v>83.318660491409105</v>
+      </c>
+      <c r="S108" s="21">
+        <v>81.912835736867137</v>
+      </c>
+      <c r="T108" s="21">
+        <v>76.400095129043336</v>
+      </c>
+      <c r="U108" s="21">
+        <v>69.233432773054901</v>
+      </c>
+      <c r="V108" s="21">
+        <v>61.890788553493145</v>
+      </c>
+    </row>
+    <row r="109" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="53" t="s">
         <v>125</v>
       </c>
@@ -6320,8 +8518,29 @@
       <c r="O109" s="17">
         <v>633.12</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P109" s="17">
+        <v>633.05999999999995</v>
+      </c>
+      <c r="Q109" s="17">
+        <v>632.85</v>
+      </c>
+      <c r="R109" s="17">
+        <v>633.26</v>
+      </c>
+      <c r="S109" s="17">
+        <v>633.38</v>
+      </c>
+      <c r="T109" s="17">
+        <v>633.70000000000005</v>
+      </c>
+      <c r="U109" s="17">
+        <v>634.61</v>
+      </c>
+      <c r="V109" s="17">
+        <v>635.16999999999996</v>
+      </c>
+    </row>
+    <row r="110" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="54">
         <v>0</v>
       </c>
@@ -6367,8 +8586,29 @@
       <c r="O110" s="21">
         <v>688.37</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P110" s="21">
+        <v>684.94</v>
+      </c>
+      <c r="Q110" s="21">
+        <v>683.03</v>
+      </c>
+      <c r="R110" s="21">
+        <v>681.85</v>
+      </c>
+      <c r="S110" s="21">
+        <v>676.03</v>
+      </c>
+      <c r="T110" s="21">
+        <v>679.66</v>
+      </c>
+      <c r="U110" s="21">
+        <v>685.1</v>
+      </c>
+      <c r="V110" s="21">
+        <v>684.48</v>
+      </c>
+    </row>
+    <row r="111" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="54">
         <v>0</v>
       </c>
@@ -6414,8 +8654,29 @@
       <c r="O111" s="21">
         <v>673.29</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P111" s="21">
+        <v>675.88</v>
+      </c>
+      <c r="Q111" s="21">
+        <v>666.83</v>
+      </c>
+      <c r="R111" s="21">
+        <v>663.13</v>
+      </c>
+      <c r="S111" s="21">
+        <v>663.26</v>
+      </c>
+      <c r="T111" s="21">
+        <v>671.44</v>
+      </c>
+      <c r="U111" s="21">
+        <v>673.89</v>
+      </c>
+      <c r="V111" s="21">
+        <v>669.36</v>
+      </c>
+    </row>
+    <row r="112" spans="1:22" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="55">
         <v>0</v>
       </c>
@@ -6461,8 +8722,29 @@
       <c r="O112" s="25">
         <v>343.74</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P112" s="25">
+        <v>343.78</v>
+      </c>
+      <c r="Q112" s="25">
+        <v>343.7</v>
+      </c>
+      <c r="R112" s="25">
+        <v>343.11</v>
+      </c>
+      <c r="S112" s="25">
+        <v>343.22</v>
+      </c>
+      <c r="T112" s="25">
+        <v>343.04</v>
+      </c>
+      <c r="U112" s="25">
+        <v>343.57</v>
+      </c>
+      <c r="V112" s="25">
+        <v>344.08</v>
+      </c>
+    </row>
+    <row r="113" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="53" t="s">
         <v>131</v>
       </c>
@@ -6508,8 +8790,29 @@
       <c r="O113" s="16">
         <v>954.19</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P113" s="16">
+        <v>934.28</v>
+      </c>
+      <c r="Q113" s="16">
+        <v>930.81</v>
+      </c>
+      <c r="R113" s="16">
+        <v>933.16</v>
+      </c>
+      <c r="S113" s="16">
+        <v>932.96</v>
+      </c>
+      <c r="T113" s="16">
+        <v>951.91</v>
+      </c>
+      <c r="U113" s="16">
+        <v>959.1</v>
+      </c>
+      <c r="V113" s="16">
+        <v>987.12</v>
+      </c>
+    </row>
+    <row r="114" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="54">
         <v>0</v>
       </c>
@@ -6555,8 +8858,29 @@
       <c r="O114" s="20">
         <v>906.06</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P114" s="20">
+        <v>887.28</v>
+      </c>
+      <c r="Q114" s="20">
+        <v>884.29</v>
+      </c>
+      <c r="R114" s="20">
+        <v>886.46</v>
+      </c>
+      <c r="S114" s="20">
+        <v>886.25</v>
+      </c>
+      <c r="T114" s="20">
+        <v>904.31</v>
+      </c>
+      <c r="U114" s="20">
+        <v>911.18</v>
+      </c>
+      <c r="V114" s="20">
+        <v>938.92</v>
+      </c>
+    </row>
+    <row r="115" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="54">
         <v>0</v>
       </c>
@@ -6602,8 +8926,29 @@
       <c r="O115" s="20">
         <v>920</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P115" s="20">
+        <v>904.52</v>
+      </c>
+      <c r="Q115" s="20">
+        <v>901.83</v>
+      </c>
+      <c r="R115" s="20">
+        <v>903.55</v>
+      </c>
+      <c r="S115" s="20">
+        <v>903.17</v>
+      </c>
+      <c r="T115" s="20">
+        <v>920.93</v>
+      </c>
+      <c r="U115" s="20">
+        <v>927.48</v>
+      </c>
+      <c r="V115" s="20">
+        <v>953.74</v>
+      </c>
+    </row>
+    <row r="116" spans="1:22" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="55">
         <v>0</v>
       </c>
@@ -6649,8 +8994,29 @@
       <c r="O116" s="24">
         <v>892.11</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P116" s="24">
+        <v>870.03</v>
+      </c>
+      <c r="Q116" s="24">
+        <v>866.74</v>
+      </c>
+      <c r="R116" s="24">
+        <v>869.37</v>
+      </c>
+      <c r="S116" s="24">
+        <v>869.34</v>
+      </c>
+      <c r="T116" s="24">
+        <v>887.69</v>
+      </c>
+      <c r="U116" s="24">
+        <v>894.87</v>
+      </c>
+      <c r="V116" s="24">
+        <v>924.09</v>
+      </c>
+    </row>
+    <row r="117" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="69" t="s">
         <v>136</v>
       </c>
@@ -6696,8 +9062,29 @@
       <c r="O117" s="17">
         <v>215.62</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P117" s="17">
+        <v>218.4</v>
+      </c>
+      <c r="Q117" s="17">
+        <v>221.04</v>
+      </c>
+      <c r="R117" s="17">
+        <v>223.36</v>
+      </c>
+      <c r="S117" s="17">
+        <v>227.53</v>
+      </c>
+      <c r="T117" s="17">
+        <v>226.66</v>
+      </c>
+      <c r="U117" s="17">
+        <v>226.58</v>
+      </c>
+      <c r="V117" s="17">
+        <v>226.79</v>
+      </c>
+    </row>
+    <row r="118" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="70">
         <v>0</v>
       </c>
@@ -6743,8 +9130,29 @@
       <c r="O118" s="21">
         <v>206.92</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P118" s="21">
+        <v>208.88</v>
+      </c>
+      <c r="Q118" s="21">
+        <v>211.98</v>
+      </c>
+      <c r="R118" s="21">
+        <v>214.92</v>
+      </c>
+      <c r="S118" s="21">
+        <v>218.5</v>
+      </c>
+      <c r="T118" s="21">
+        <v>216.47</v>
+      </c>
+      <c r="U118" s="21">
+        <v>217.23</v>
+      </c>
+      <c r="V118" s="21">
+        <v>217.48</v>
+      </c>
+    </row>
+    <row r="119" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="70">
         <v>0</v>
       </c>
@@ -6790,8 +9198,29 @@
       <c r="O119" s="21">
         <v>213.47</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P119" s="21">
+        <v>217.44</v>
+      </c>
+      <c r="Q119" s="21">
+        <v>219.31</v>
+      </c>
+      <c r="R119" s="21">
+        <v>221.9</v>
+      </c>
+      <c r="S119" s="21">
+        <v>225.12</v>
+      </c>
+      <c r="T119" s="21">
+        <v>224.33</v>
+      </c>
+      <c r="U119" s="21">
+        <v>224.85</v>
+      </c>
+      <c r="V119" s="21">
+        <v>224.68</v>
+      </c>
+    </row>
+    <row r="120" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="70">
         <v>0</v>
       </c>
@@ -6837,8 +9266,29 @@
       <c r="O120" s="21">
         <v>214.07</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P120" s="21">
+        <v>214.53</v>
+      </c>
+      <c r="Q120" s="21">
+        <v>218.3</v>
+      </c>
+      <c r="R120" s="21">
+        <v>218</v>
+      </c>
+      <c r="S120" s="21">
+        <v>222.58</v>
+      </c>
+      <c r="T120" s="21">
+        <v>223.94</v>
+      </c>
+      <c r="U120" s="21">
+        <v>222.93</v>
+      </c>
+      <c r="V120" s="21">
+        <v>222.66</v>
+      </c>
+    </row>
+    <row r="121" spans="1:22" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A121" s="71">
         <v>0</v>
       </c>
@@ -6884,8 +9334,29 @@
       <c r="O121" s="25">
         <v>97.92</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P121" s="25">
+        <v>98.68</v>
+      </c>
+      <c r="Q121" s="25">
+        <v>98.68</v>
+      </c>
+      <c r="R121" s="25">
+        <v>98.68</v>
+      </c>
+      <c r="S121" s="25">
+        <v>98.68</v>
+      </c>
+      <c r="T121" s="25">
+        <v>98.02</v>
+      </c>
+      <c r="U121" s="25">
+        <v>97.02</v>
+      </c>
+      <c r="V121" s="25">
+        <v>94.04</v>
+      </c>
+    </row>
+    <row r="122" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="53" t="s">
         <v>142</v>
       </c>
@@ -6931,8 +9402,29 @@
       <c r="O122" s="21">
         <v>223.46</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P122" s="21">
+        <v>227.55</v>
+      </c>
+      <c r="Q122" s="21">
+        <v>226.56</v>
+      </c>
+      <c r="R122" s="21">
+        <v>229.79</v>
+      </c>
+      <c r="S122" s="21">
+        <v>232.04</v>
+      </c>
+      <c r="T122" s="21">
+        <v>231.78</v>
+      </c>
+      <c r="U122" s="21">
+        <v>233.27</v>
+      </c>
+      <c r="V122" s="21">
+        <v>233.29</v>
+      </c>
+    </row>
+    <row r="123" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="54">
         <v>0</v>
       </c>
@@ -6978,8 +9470,29 @@
       <c r="O123" s="21">
         <v>214.7</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P123" s="21">
+        <v>217.84</v>
+      </c>
+      <c r="Q123" s="21">
+        <v>220.36</v>
+      </c>
+      <c r="R123" s="21">
+        <v>221.88</v>
+      </c>
+      <c r="S123" s="21">
+        <v>222.83</v>
+      </c>
+      <c r="T123" s="21">
+        <v>223.06</v>
+      </c>
+      <c r="U123" s="21">
+        <v>226.71</v>
+      </c>
+      <c r="V123" s="21">
+        <v>225.59</v>
+      </c>
+    </row>
+    <row r="124" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="54">
         <v>0</v>
       </c>
@@ -7025,8 +9538,29 @@
       <c r="O124" s="21">
         <v>223.91</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P124" s="21">
+        <v>228.06</v>
+      </c>
+      <c r="Q124" s="21">
+        <v>226.89</v>
+      </c>
+      <c r="R124" s="21">
+        <v>230.2</v>
+      </c>
+      <c r="S124" s="21">
+        <v>232.52</v>
+      </c>
+      <c r="T124" s="21">
+        <v>232.23</v>
+      </c>
+      <c r="U124" s="21">
+        <v>233.62</v>
+      </c>
+      <c r="V124" s="21">
+        <v>233.7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="54">
         <v>0</v>
       </c>
@@ -7072,8 +9606,29 @@
       <c r="O125" s="21">
         <v>217.69</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P125" s="21">
+        <v>219.48</v>
+      </c>
+      <c r="Q125" s="21">
+        <v>219.22</v>
+      </c>
+      <c r="R125" s="21">
+        <v>217.5</v>
+      </c>
+      <c r="S125" s="21">
+        <v>220.31</v>
+      </c>
+      <c r="T125" s="21">
+        <v>219.96</v>
+      </c>
+      <c r="U125" s="21">
+        <v>220.2</v>
+      </c>
+      <c r="V125" s="21">
+        <v>221.51</v>
+      </c>
+    </row>
+    <row r="126" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="54">
         <v>0</v>
       </c>
@@ -7119,8 +9674,29 @@
       <c r="O126" s="21">
         <v>481.53</v>
       </c>
-    </row>
-    <row r="127" spans="1:15" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P126" s="21">
+        <v>482.76</v>
+      </c>
+      <c r="Q126" s="21">
+        <v>483.28</v>
+      </c>
+      <c r="R126" s="21">
+        <v>484.38</v>
+      </c>
+      <c r="S126" s="21">
+        <v>487.6</v>
+      </c>
+      <c r="T126" s="21">
+        <v>487.05</v>
+      </c>
+      <c r="U126" s="21">
+        <v>486.02</v>
+      </c>
+      <c r="V126" s="21">
+        <v>490.21</v>
+      </c>
+    </row>
+    <row r="127" spans="1:22" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="54"/>
       <c r="B127" s="18" t="s">
         <v>147</v>
@@ -7164,8 +9740,29 @@
       <c r="O127" s="21">
         <v>272.08999999999997</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P127" s="21">
+        <v>270.18</v>
+      </c>
+      <c r="Q127" s="21">
+        <v>265.7</v>
+      </c>
+      <c r="R127" s="21">
+        <v>269.17</v>
+      </c>
+      <c r="S127" s="21">
+        <v>264.48</v>
+      </c>
+      <c r="T127" s="21">
+        <v>264.48</v>
+      </c>
+      <c r="U127" s="21">
+        <v>242.04</v>
+      </c>
+      <c r="V127" s="21">
+        <v>236.26</v>
+      </c>
+    </row>
+    <row r="128" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="54"/>
       <c r="B128" s="18" t="s">
         <v>147</v>
@@ -7209,8 +9806,29 @@
       <c r="O128" s="21">
         <v>2.12</v>
       </c>
-    </row>
-    <row r="129" spans="1:15" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P128" s="21">
+        <v>2.11</v>
+      </c>
+      <c r="Q128" s="21">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="R128" s="21">
+        <v>2.09</v>
+      </c>
+      <c r="S128" s="21">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="T128" s="21">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="U128" s="21">
+        <v>1.88</v>
+      </c>
+      <c r="V128" s="21">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="129" spans="1:22" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="54">
         <v>0</v>
       </c>
@@ -7256,8 +9874,29 @@
       <c r="O129" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="130" spans="1:15" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P129" s="21">
+        <v>1.98</v>
+      </c>
+      <c r="Q129" s="21">
+        <v>1.95</v>
+      </c>
+      <c r="R129" s="21">
+        <v>1.98</v>
+      </c>
+      <c r="S129" s="21">
+        <v>1.95</v>
+      </c>
+      <c r="T129" s="21">
+        <v>1.95</v>
+      </c>
+      <c r="U129" s="21">
+        <v>1.78</v>
+      </c>
+      <c r="V129" s="21">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="130" spans="1:22" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="54"/>
       <c r="B130" s="18" t="s">
         <v>147</v>
@@ -7301,8 +9940,29 @@
       <c r="O130" s="21">
         <v>293.45</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P130" s="21">
+        <v>289.07</v>
+      </c>
+      <c r="Q130" s="21">
+        <v>284.8</v>
+      </c>
+      <c r="R130" s="21">
+        <v>287.49</v>
+      </c>
+      <c r="S130" s="21">
+        <v>282.72000000000003</v>
+      </c>
+      <c r="T130" s="21">
+        <v>285.70999999999998</v>
+      </c>
+      <c r="U130" s="21">
+        <v>259.61</v>
+      </c>
+      <c r="V130" s="21">
+        <v>245.01</v>
+      </c>
+    </row>
+    <row r="131" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="54"/>
       <c r="B131" s="18" t="s">
         <v>147</v>
@@ -7346,8 +10006,29 @@
       <c r="O131" s="21">
         <v>2.3199999999999998</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P131" s="21">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="Q131" s="21">
+        <v>2.23</v>
+      </c>
+      <c r="R131" s="21">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="S131" s="21">
+        <v>2.21</v>
+      </c>
+      <c r="T131" s="21">
+        <v>2.25</v>
+      </c>
+      <c r="U131" s="21">
+        <v>2.04</v>
+      </c>
+      <c r="V131" s="21">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="132" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="54"/>
       <c r="B132" s="18" t="s">
         <v>147</v>
@@ -7391,8 +10072,29 @@
       <c r="O132" s="21">
         <v>2.12</v>
       </c>
-    </row>
-    <row r="133" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P132" s="21">
+        <v>2.09</v>
+      </c>
+      <c r="Q132" s="21">
+        <v>2.08</v>
+      </c>
+      <c r="R132" s="21">
+        <v>2.09</v>
+      </c>
+      <c r="S132" s="21">
+        <v>2.06</v>
+      </c>
+      <c r="T132" s="21">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="U132" s="21">
+        <v>1.89</v>
+      </c>
+      <c r="V132" s="21">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="133" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="54"/>
       <c r="B133" s="18" t="s">
         <v>147</v>
@@ -7436,8 +10138,29 @@
       <c r="O133" s="21">
         <v>289.3</v>
       </c>
-    </row>
-    <row r="134" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P133" s="21">
+        <v>285.74</v>
+      </c>
+      <c r="Q133" s="21">
+        <v>282.23</v>
+      </c>
+      <c r="R133" s="21">
+        <v>276.3</v>
+      </c>
+      <c r="S133" s="21">
+        <v>276.64</v>
+      </c>
+      <c r="T133" s="21">
+        <v>276.64</v>
+      </c>
+      <c r="U133" s="21">
+        <v>278.47000000000003</v>
+      </c>
+      <c r="V133" s="21">
+        <v>273.48</v>
+      </c>
+    </row>
+    <row r="134" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="54"/>
       <c r="B134" s="18" t="s">
         <v>147</v>
@@ -7481,8 +10204,29 @@
       <c r="O134" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="135" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P134" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q134" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R134" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="S134" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T134" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U134" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V134" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="135" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="54"/>
       <c r="B135" s="18" t="s">
         <v>147</v>
@@ -7526,8 +10270,29 @@
       <c r="O135" s="21">
         <v>400.35</v>
       </c>
-    </row>
-    <row r="136" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P135" s="21">
+        <v>401.28</v>
+      </c>
+      <c r="Q135" s="21">
+        <v>394.36</v>
+      </c>
+      <c r="R135" s="21">
+        <v>391.64</v>
+      </c>
+      <c r="S135" s="21">
+        <v>391.64</v>
+      </c>
+      <c r="T135" s="21">
+        <v>391.64</v>
+      </c>
+      <c r="U135" s="21">
+        <v>384.56</v>
+      </c>
+      <c r="V135" s="21">
+        <v>379.16</v>
+      </c>
+    </row>
+    <row r="136" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="54"/>
       <c r="B136" s="18" t="s">
         <v>147</v>
@@ -7571,8 +10336,29 @@
       <c r="O136" s="21">
         <v>3.06</v>
       </c>
-    </row>
-    <row r="137" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P136" s="21">
+        <v>3.06</v>
+      </c>
+      <c r="Q136" s="21">
+        <v>3.02</v>
+      </c>
+      <c r="R136" s="21">
+        <v>3.01</v>
+      </c>
+      <c r="S136" s="21">
+        <v>3.01</v>
+      </c>
+      <c r="T136" s="21">
+        <v>3.01</v>
+      </c>
+      <c r="U136" s="21">
+        <v>2.94</v>
+      </c>
+      <c r="V136" s="21">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="54"/>
       <c r="B137" s="18" t="s">
         <v>147</v>
@@ -7616,8 +10402,29 @@
       <c r="O137" s="21">
         <v>3</v>
       </c>
-    </row>
-    <row r="138" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P137" s="21">
+        <v>3.01</v>
+      </c>
+      <c r="Q137" s="21">
+        <v>2.95</v>
+      </c>
+      <c r="R137" s="21">
+        <v>2.91</v>
+      </c>
+      <c r="S137" s="21">
+        <v>2.91</v>
+      </c>
+      <c r="T137" s="21">
+        <v>2.91</v>
+      </c>
+      <c r="U137" s="21">
+        <v>2.88</v>
+      </c>
+      <c r="V137" s="21">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="138" spans="1:22" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A138" s="55">
         <v>0</v>
       </c>
@@ -7663,8 +10470,29 @@
       <c r="O138" s="21">
         <v>251.32</v>
       </c>
-    </row>
-    <row r="139" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P138" s="21">
+        <v>251.44</v>
+      </c>
+      <c r="Q138" s="21">
+        <v>251.46</v>
+      </c>
+      <c r="R138" s="21">
+        <v>251.44</v>
+      </c>
+      <c r="S138" s="21">
+        <v>251.43</v>
+      </c>
+      <c r="T138" s="21">
+        <v>251.42</v>
+      </c>
+      <c r="U138" s="21">
+        <v>251.45</v>
+      </c>
+      <c r="V138" s="21">
+        <v>251.44</v>
+      </c>
+    </row>
+    <row r="139" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="53" t="s">
         <v>152</v>
       </c>
@@ -7710,8 +10538,29 @@
       <c r="O139" s="17">
         <v>89.47</v>
       </c>
-    </row>
-    <row r="140" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P139" s="17">
+        <v>92.04</v>
+      </c>
+      <c r="Q139" s="17">
+        <v>89.74</v>
+      </c>
+      <c r="R139" s="17">
+        <v>98.35</v>
+      </c>
+      <c r="S139" s="17">
+        <v>88.14</v>
+      </c>
+      <c r="T139" s="17">
+        <v>88.57</v>
+      </c>
+      <c r="U139" s="17">
+        <v>91.49</v>
+      </c>
+      <c r="V139" s="17">
+        <v>89.51</v>
+      </c>
+    </row>
+    <row r="140" spans="1:22" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="54"/>
       <c r="B140" s="18" t="s">
         <v>153</v>
@@ -7755,8 +10604,29 @@
       <c r="O140" s="21">
         <v>796.86</v>
       </c>
-    </row>
-    <row r="141" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P140" s="21">
+        <v>782.66</v>
+      </c>
+      <c r="Q140" s="21">
+        <v>785.11</v>
+      </c>
+      <c r="R140" s="21">
+        <v>798.69</v>
+      </c>
+      <c r="S140" s="21">
+        <v>773.91</v>
+      </c>
+      <c r="T140" s="21">
+        <v>780.87</v>
+      </c>
+      <c r="U140" s="21">
+        <v>788.67</v>
+      </c>
+      <c r="V140" s="21">
+        <v>781.33</v>
+      </c>
+    </row>
+    <row r="141" spans="1:22" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A141" s="55">
         <v>0</v>
       </c>
@@ -7802,11 +10672,32 @@
       <c r="O141" s="25">
         <v>260.99</v>
       </c>
-    </row>
-    <row r="142" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P141" s="25">
+        <v>262.51</v>
+      </c>
+      <c r="Q141" s="25">
+        <v>261.13</v>
+      </c>
+      <c r="R141" s="25">
+        <v>257.57</v>
+      </c>
+      <c r="S141" s="25">
+        <v>253.67</v>
+      </c>
+      <c r="T141" s="25">
+        <v>253.23</v>
+      </c>
+      <c r="U141" s="25">
+        <v>251.16</v>
+      </c>
+      <c r="V141" s="25">
+        <v>244.78</v>
+      </c>
+    </row>
+    <row r="142" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B142" s="46"/>
     </row>
-    <row r="143" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:22" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="56" t="s">
         <v>2</v>
       </c>
@@ -7824,8 +10715,15 @@
       <c r="M143" s="48"/>
       <c r="N143" s="48"/>
       <c r="O143" s="48"/>
-    </row>
-    <row r="144" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P143" s="48"/>
+      <c r="Q143" s="48"/>
+      <c r="R143" s="48"/>
+      <c r="S143" s="48"/>
+      <c r="T143" s="48"/>
+      <c r="U143" s="48"/>
+      <c r="V143" s="48"/>
+    </row>
+    <row r="144" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="56"/>
       <c r="B144" s="56"/>
       <c r="C144" s="56"/>
@@ -7841,8 +10739,15 @@
       <c r="M144" s="48"/>
       <c r="N144" s="48"/>
       <c r="O144" s="48"/>
-    </row>
-    <row r="145" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P144" s="48"/>
+      <c r="Q144" s="48"/>
+      <c r="R144" s="48"/>
+      <c r="S144" s="48"/>
+      <c r="T144" s="48"/>
+      <c r="U144" s="48"/>
+      <c r="V144" s="48"/>
+    </row>
+    <row r="145" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="56"/>
       <c r="B145" s="56"/>
       <c r="C145" s="56"/>
@@ -7858,8 +10763,15 @@
       <c r="M145" s="48"/>
       <c r="N145" s="48"/>
       <c r="O145" s="48"/>
-    </row>
-    <row r="146" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P145" s="48"/>
+      <c r="Q145" s="48"/>
+      <c r="R145" s="48"/>
+      <c r="S145" s="48"/>
+      <c r="T145" s="48"/>
+      <c r="U145" s="48"/>
+      <c r="V145" s="48"/>
+    </row>
+    <row r="146" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="56"/>
       <c r="B146" s="56"/>
       <c r="C146" s="56"/>
@@ -7875,8 +10787,15 @@
       <c r="M146" s="48"/>
       <c r="N146" s="48"/>
       <c r="O146" s="48"/>
-    </row>
-    <row r="147" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P146" s="48"/>
+      <c r="Q146" s="48"/>
+      <c r="R146" s="48"/>
+      <c r="S146" s="48"/>
+      <c r="T146" s="48"/>
+      <c r="U146" s="48"/>
+      <c r="V146" s="48"/>
+    </row>
+    <row r="147" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="56"/>
       <c r="B147" s="56"/>
       <c r="C147" s="56"/>
@@ -7892,8 +10811,15 @@
       <c r="M147" s="47"/>
       <c r="N147" s="47"/>
       <c r="O147" s="47"/>
-    </row>
-    <row r="148" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P147" s="47"/>
+      <c r="Q147" s="47"/>
+      <c r="R147" s="47"/>
+      <c r="S147" s="47"/>
+      <c r="T147" s="47"/>
+      <c r="U147" s="47"/>
+      <c r="V147" s="47"/>
+    </row>
+    <row r="148" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="56"/>
       <c r="B148" s="56"/>
       <c r="C148" s="56"/>
@@ -7909,8 +10835,15 @@
       <c r="M148" s="47"/>
       <c r="N148" s="47"/>
       <c r="O148" s="47"/>
-    </row>
-    <row r="149" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P148" s="47"/>
+      <c r="Q148" s="47"/>
+      <c r="R148" s="47"/>
+      <c r="S148" s="47"/>
+      <c r="T148" s="47"/>
+      <c r="U148" s="47"/>
+      <c r="V148" s="47"/>
+    </row>
+    <row r="149" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="56"/>
       <c r="B149" s="56"/>
       <c r="C149" s="56"/>
@@ -7926,36 +10859,43 @@
       <c r="M149" s="47"/>
       <c r="N149" s="47"/>
       <c r="O149" s="47"/>
-    </row>
-    <row r="150" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P149" s="47"/>
+      <c r="Q149" s="47"/>
+      <c r="R149" s="47"/>
+      <c r="S149" s="47"/>
+      <c r="T149" s="47"/>
+      <c r="U149" s="47"/>
+      <c r="V149" s="47"/>
+    </row>
+    <row r="150" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="56"/>
       <c r="B150" s="56"/>
       <c r="C150" s="56"/>
     </row>
-    <row r="151" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="48"/>
       <c r="B151" s="48"/>
       <c r="C151" s="48"/>
     </row>
-    <row r="152" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="153" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="154" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="155" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="156" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="157" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="158" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="159" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="160" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="161" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="162" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="163" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="164" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="165" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="166" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="167" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="168" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="169" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="170" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="152" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="153" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="154" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="155" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="156" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="157" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="158" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="159" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="160" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="161" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="162" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="163" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="164" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="165" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="166" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="167" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="168" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="169" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="170" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A139:A141"/>

</xml_diff>